<commit_message>
[Silverfox] Tube Data 분리에 따라 cid 정리
</commit_message>
<xml_diff>
--- a/DesignDocs/VariableData/TubeCooler.xlsx
+++ b/DesignDocs/VariableData/TubeCooler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\VariableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D15548B-8794-4639-B16B-CBF7733DE0CE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0C72FB-8CDB-4BC1-A9DC-ABF8E674C75B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="8115" xr2:uid="{F598384B-001D-4AD5-B5A5-EB89C313FEFA}"/>
   </bookViews>
@@ -581,7 +581,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -732,7 +732,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>5102</v>
+        <v>7101</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>5105</v>
+        <v>7102</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
@@ -778,7 +778,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>5108</v>
+        <v>7103</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>5111</v>
+        <v>7104</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>5114</v>
+        <v>7105</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>5117</v>
+        <v>7106</v>
       </c>
       <c r="B12" t="s">
         <v>35</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>5300</v>
+        <v>7107</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>5301</v>
+        <v>7108</v>
       </c>
       <c r="B14" t="s">
         <v>39</v>

</xml_diff>